<commit_message>
bætt við gröfum í Mælingar excel skjal
</commit_message>
<xml_diff>
--- a/KodaVinnsla/Maelingar/Hitamælingar_með_viftu.xlsx
+++ b/KodaVinnsla/Maelingar/Hitamælingar_með_viftu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rúnar U\Documents\Skóli\Tölvunarfræði\Örtölvu- og mælitækni\Hópverkefni - Hönnun\H-nnunarverkefni-rt-lvu-og-m-lit-kni-2020\KodaVinnsla\Maelingar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D43FC6-B79D-45C0-909D-27D0FB2D5F6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C92A33D8-F4A2-4E35-BB08-530095A54164}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>tími</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>jafnvægishitastig</t>
+  </si>
+  <si>
+    <t>Jafnvhitastig án viftu:</t>
   </si>
 </sst>
 </file>
@@ -5036,34 +5039,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="log"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$G$28:$G$38</c:f>
@@ -5459,6 +5434,542 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Jafnvægishitastig sem fall af duty cycle á línulegu sviði</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="10"/>
+            <c:backward val="10"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.0020833333333333E-2"/>
+                  <c:y val="-0.40268675055323966"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$29:$G$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$29:$J$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>28.35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23.209999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.86</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.310000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23.699999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22.61</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23.649999999999995</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22.87</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.219999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-043A-49F7-88EA-3BDBCB32664F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="435417088"/>
+        <c:axId val="251843536"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="435417088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Duty</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> cycle</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="251843536"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="251843536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="30"/>
+          <c:min val="20"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Hitastig (°C)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="435417088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -5500,6 +6011,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -6571,6 +7122,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -6640,6 +7707,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CEBD7E4-4810-4D08-99B7-9514B4CA5FA1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6913,8 +8018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N631"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R66" sqref="R66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7537,6 +8642,13 @@
         <f t="shared" si="1"/>
         <v>23.86</v>
       </c>
+      <c r="L31" t="s">
+        <v>11</v>
+      </c>
+      <c r="N31">
+        <f>_xlfn.MAXIFS($F$2:$F$631,$C$2:$C$631,0,$D$2:$D$631,0)</f>
+        <v>75.799999999999983</v>
+      </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32">

</xml_diff>

<commit_message>
mælingarkóða breytt til að taka bara 10% og 90% gildi
</commit_message>
<xml_diff>
--- a/KodaVinnsla/Maelingar/Hitamælingar_með_viftu.xlsx
+++ b/KodaVinnsla/Maelingar/Hitamælingar_með_viftu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rúnar U\Documents\Skóli\Tölvunarfræði\Örtölvu- og mælitækni\Hópverkefni - Hönnun\H-nnunarverkefni-rt-lvu-og-m-lit-kni-2020\KodaVinnsla\Maelingar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C92A33D8-F4A2-4E35-BB08-530095A54164}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FE19B5-E250-48D7-AF9E-995F96DAD7F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,8 +33,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>tími</t>
   </si>
@@ -70,6 +92,18 @@
   </si>
   <si>
     <t>Jafnvhitastig án viftu:</t>
+  </si>
+  <si>
+    <t>fan_on</t>
+  </si>
+  <si>
+    <t>jafnv. Hiti</t>
+  </si>
+  <si>
+    <t>tímastuðull</t>
+  </si>
+  <si>
+    <t>63% hitabr.</t>
   </si>
 </sst>
 </file>
@@ -8016,10 +8050,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N631"/>
+  <dimension ref="A1:Y631"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R66" sqref="R66"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8303,7 +8337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>28.14</v>
       </c>
@@ -8320,7 +8354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>29.58</v>
       </c>
@@ -8337,7 +8371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>30.58</v>
       </c>
@@ -8354,7 +8388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>32.01</v>
       </c>
@@ -8371,7 +8405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>33.01</v>
       </c>
@@ -8388,7 +8422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>34.450000000000003</v>
       </c>
@@ -8405,7 +8439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>35.450000000000003</v>
       </c>
@@ -8422,7 +8456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>36.89</v>
       </c>
@@ -8439,7 +8473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>37.89</v>
       </c>
@@ -8456,7 +8490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>39.32</v>
       </c>
@@ -8476,7 +8510,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>40.33</v>
       </c>
@@ -8501,8 +8535,26 @@
       <c r="J27" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="T27" t="s">
+        <v>12</v>
+      </c>
+      <c r="U27" t="s">
+        <v>7</v>
+      </c>
+      <c r="V27" t="s">
+        <v>6</v>
+      </c>
+      <c r="W27" t="s">
+        <v>13</v>
+      </c>
+      <c r="X27" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>41.77</v>
       </c>
@@ -8533,8 +8585,22 @@
         <f>_xlfn.MAXIFS($F$2:$F$631,$C$2:$C$631,1,$D$2:$D$631,G28)</f>
         <v>67.800000000000011</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <v>0</v>
+      </c>
+      <c r="V28" cm="1">
+        <f t="array" ref="V28:V38">H28:H38</f>
+        <v>393.48</v>
+      </c>
+      <c r="W28">
+        <f>N31</f>
+        <v>75.799999999999983</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>42.77</v>
       </c>
@@ -8572,8 +8638,30 @@
         <f>CEILING(MAX($B$2:$B$631),10)</f>
         <v>80</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="T29">
+        <v>1</v>
+      </c>
+      <c r="U29">
+        <f>G28</f>
+        <v>0</v>
+      </c>
+      <c r="V29">
+        <v>478.38</v>
+      </c>
+      <c r="W29">
+        <f>J28</f>
+        <v>67.800000000000011</v>
+      </c>
+      <c r="X29">
+        <f>W28-0.63*(W28-W29)</f>
+        <v>70.760000000000005</v>
+      </c>
+      <c r="Y29">
+        <f>_xlfn.MINIFS($A$2:$A$631,$B$2:$B$631, "&lt;"&amp; W29, $C$2:$C$631,T29,$D$2:$D$631,U29)-V28</f>
+        <v>80.089999999999975</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>44.2</v>
       </c>
@@ -8610,8 +8698,30 @@
       <c r="N30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="T30">
+        <v>1</v>
+      </c>
+      <c r="U30">
+        <f t="shared" ref="U30:U38" si="3">G29</f>
+        <v>10</v>
+      </c>
+      <c r="V30">
+        <v>692.88</v>
+      </c>
+      <c r="W30">
+        <f t="shared" ref="W30:W39" si="4">J29</f>
+        <v>28.35</v>
+      </c>
+      <c r="X30">
+        <f t="shared" ref="X30:X39" si="5">W29-0.63*(W29-W30)</f>
+        <v>42.9465</v>
+      </c>
+      <c r="Y30">
+        <f t="shared" ref="Y30:Y39" si="6">_xlfn.MINIFS($A$2:$A$631,$B$2:$B$631, "&lt;"&amp; W30, $C$2:$C$631,T30,$D$2:$D$631,U30)-V29</f>
+        <v>201.47000000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>45.2</v>
       </c>
@@ -8649,8 +8759,30 @@
         <f>_xlfn.MAXIFS($F$2:$F$631,$C$2:$C$631,0,$D$2:$D$631,0)</f>
         <v>75.799999999999983</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="T31">
+        <v>1</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="V31">
+        <v>930.26</v>
+      </c>
+      <c r="W31">
+        <f t="shared" si="4"/>
+        <v>23.209999999999997</v>
+      </c>
+      <c r="X31">
+        <f t="shared" si="5"/>
+        <v>25.111799999999999</v>
+      </c>
+      <c r="Y31">
+        <f t="shared" si="6"/>
+        <v>224.21000000000004</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>46.64</v>
       </c>
@@ -8681,8 +8813,30 @@
         <f t="shared" si="1"/>
         <v>24.310000000000002</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="T32">
+        <v>1</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="V32">
+        <v>961.72</v>
+      </c>
+      <c r="W32">
+        <f t="shared" si="4"/>
+        <v>23.86</v>
+      </c>
+      <c r="X32">
+        <f t="shared" si="5"/>
+        <v>23.619499999999999</v>
+      </c>
+      <c r="Y32">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>47.64</v>
       </c>
@@ -8713,8 +8867,30 @@
         <f t="shared" si="1"/>
         <v>23.699999999999996</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="T33">
+        <v>1</v>
+      </c>
+      <c r="U33">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="V33">
+        <v>993.32</v>
+      </c>
+      <c r="W33">
+        <f t="shared" si="4"/>
+        <v>24.310000000000002</v>
+      </c>
+      <c r="X33">
+        <f t="shared" si="5"/>
+        <v>24.1435</v>
+      </c>
+      <c r="Y33">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>48.98</v>
       </c>
@@ -8745,8 +8921,30 @@
         <f t="shared" si="1"/>
         <v>22.61</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="T34">
+        <v>1</v>
+      </c>
+      <c r="U34">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="V34">
+        <v>1050.43</v>
+      </c>
+      <c r="W34">
+        <f t="shared" si="4"/>
+        <v>23.699999999999996</v>
+      </c>
+      <c r="X34">
+        <f t="shared" si="5"/>
+        <v>23.925699999999999</v>
+      </c>
+      <c r="Y34">
+        <f t="shared" si="6"/>
+        <v>54.669999999999959</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>49.98</v>
       </c>
@@ -8777,8 +8975,30 @@
         <f t="shared" si="1"/>
         <v>23.649999999999995</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="T35">
+        <v>1</v>
+      </c>
+      <c r="U35">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="V35">
+        <v>1090.3399999999999</v>
+      </c>
+      <c r="W35">
+        <f t="shared" si="4"/>
+        <v>22.61</v>
+      </c>
+      <c r="X35">
+        <f t="shared" si="5"/>
+        <v>23.013299999999997</v>
+      </c>
+      <c r="Y35">
+        <f t="shared" si="6"/>
+        <v>31.589999999999918</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>51.42</v>
       </c>
@@ -8809,8 +9029,30 @@
         <f t="shared" si="1"/>
         <v>22.87</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="T36">
+        <v>1</v>
+      </c>
+      <c r="U36">
+        <f t="shared" si="3"/>
+        <v>70</v>
+      </c>
+      <c r="V36">
+        <v>1126.72</v>
+      </c>
+      <c r="W36">
+        <f t="shared" si="4"/>
+        <v>23.649999999999995</v>
+      </c>
+      <c r="X36">
+        <f t="shared" si="5"/>
+        <v>23.265199999999997</v>
+      </c>
+      <c r="Y36">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>52.42</v>
       </c>
@@ -8841,8 +9083,30 @@
         <f t="shared" si="1"/>
         <v>23.219999999999995</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="T37">
+        <v>1</v>
+      </c>
+      <c r="U37">
+        <f t="shared" si="3"/>
+        <v>80</v>
+      </c>
+      <c r="V37">
+        <v>1160.6300000000001</v>
+      </c>
+      <c r="W37">
+        <f t="shared" si="4"/>
+        <v>22.87</v>
+      </c>
+      <c r="X37">
+        <f t="shared" si="5"/>
+        <v>23.1586</v>
+      </c>
+      <c r="Y37">
+        <f t="shared" si="6"/>
+        <v>28.029999999999973</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>53.75</v>
       </c>
@@ -8873,8 +9137,30 @@
         <f t="shared" si="1"/>
         <v>21.759999999999994</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="T38">
+        <v>1</v>
+      </c>
+      <c r="U38">
+        <f t="shared" si="3"/>
+        <v>90</v>
+      </c>
+      <c r="V38">
+        <v>1192.02</v>
+      </c>
+      <c r="W38">
+        <f t="shared" si="4"/>
+        <v>23.219999999999995</v>
+      </c>
+      <c r="X38">
+        <f t="shared" si="5"/>
+        <v>23.090499999999999</v>
+      </c>
+      <c r="Y38">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>54.75</v>
       </c>
@@ -8890,8 +9176,31 @@
       <c r="E39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="T39">
+        <v>1</v>
+      </c>
+      <c r="U39">
+        <f>G38</f>
+        <v>100</v>
+      </c>
+      <c r="V39">
+        <f>MAX($A$2:$A$631)</f>
+        <v>1240.6500000000001</v>
+      </c>
+      <c r="W39">
+        <f t="shared" si="4"/>
+        <v>21.759999999999994</v>
+      </c>
+      <c r="X39">
+        <f t="shared" si="5"/>
+        <v>22.300199999999993</v>
+      </c>
+      <c r="Y39">
+        <f t="shared" si="6"/>
+        <v>42.759999999999991</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>56.18</v>
       </c>
@@ -8908,7 +9217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>57.18</v>
       </c>
@@ -8925,7 +9234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>58.62</v>
       </c>
@@ -8942,7 +9251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>59.62</v>
       </c>
@@ -8959,7 +9268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>61.06</v>
       </c>
@@ -8976,7 +9285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>62.06</v>
       </c>
@@ -8993,7 +9302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>63.49</v>
       </c>
@@ -9010,7 +9319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>64.489999999999995</v>
       </c>
@@ -9027,7 +9336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>85.08</v>
       </c>

</xml_diff>

<commit_message>
Fleiri mælingar á hita og viftu
</commit_message>
<xml_diff>
--- a/KodaVinnsla/Maelingar/Hitamælingar_með_viftu.xlsx
+++ b/KodaVinnsla/Maelingar/Hitamælingar_með_viftu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rúnar U\Documents\Skóli\Tölvunarfræði\Örtölvu- og mælitækni\Hópverkefni - Hönnun\H-nnunarverkefni-rt-lvu-og-m-lit-kni-2020\KodaVinnsla\Maelingar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FE19B5-E250-48D7-AF9E-995F96DAD7F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81AE0E3-5027-42A9-B707-DF41628BA328}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8052,8 +8052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y631"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>